<commit_message>
Atualização automática 2026-02-20 11:00:37.943269
</commit_message>
<xml_diff>
--- a/Monitores.xlsx
+++ b/Monitores.xlsx
@@ -16,17 +16,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +36,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +44,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,37 +435,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Serial</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Fabricante</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Total de manutenções</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Última atualização</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Computador conectado</t>
         </is>
@@ -503,10 +495,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-08-27T16:52:20</t>
-        </is>
+      <c r="F2" s="2" t="n">
+        <v>45896.70300925926</v>
       </c>
     </row>
     <row r="3">
@@ -533,10 +523,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2026-02-19T23:41:47</t>
-        </is>
+      <c r="F3" s="2" t="n">
+        <v>46072.98734953703</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -568,10 +556,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2026-01-09T10:27:20</t>
-        </is>
+      <c r="F4" s="2" t="n">
+        <v>46031.43564814814</v>
       </c>
     </row>
     <row r="5">
@@ -598,10 +584,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-08-12T09:04:31</t>
-        </is>
+      <c r="F5" s="2" t="n">
+        <v>45881.37813657407</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -633,10 +617,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-11-10T07:50:50</t>
-        </is>
+      <c r="F6" s="2" t="n">
+        <v>45971.32696759259</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -668,10 +650,8 @@
           <t>Em manutenção</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-10-03T11:22:32</t>
-        </is>
+      <c r="F7" s="2" t="n">
+        <v>45933.47398148148</v>
       </c>
     </row>
     <row r="8">
@@ -698,10 +678,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2026-02-20T09:08:42</t>
-        </is>
+      <c r="F8" s="2" t="n">
+        <v>46073.38104166667</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -733,10 +711,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2026-02-20T08:54:23</t>
-        </is>
+      <c r="F9" s="2" t="n">
+        <v>46073.37109953703</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -768,10 +744,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2026-01-16T15:43:06</t>
-        </is>
+      <c r="F10" s="2" t="n">
+        <v>46038.65493055555</v>
       </c>
     </row>
     <row r="11">
@@ -798,10 +772,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2025-08-08T15:25:45</t>
-        </is>
+      <c r="F11" s="2" t="n">
+        <v>45877.64288194444</v>
       </c>
     </row>
     <row r="12">
@@ -828,10 +800,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2025-12-11T09:08:24</t>
-        </is>
+      <c r="F12" s="2" t="n">
+        <v>46002.38083333334</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -863,10 +833,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2026-01-26T15:36:32</t>
-        </is>
+      <c r="F13" s="2" t="n">
+        <v>46048.65037037037</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -898,10 +866,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2025-07-31T08:28:57</t>
-        </is>
+      <c r="F14" s="2" t="n">
+        <v>45869.3534375</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -933,10 +899,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2025-12-15T11:02:24</t>
-        </is>
+      <c r="F15" s="2" t="n">
+        <v>46006.46</v>
       </c>
     </row>
     <row r="16">
@@ -963,10 +927,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2025-12-22T12:15:14</t>
-        </is>
+      <c r="F16" s="2" t="n">
+        <v>46013.5105787037</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -998,10 +960,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2026-02-20T07:15:02</t>
-        </is>
+      <c r="F17" s="2" t="n">
+        <v>46073.30210648148</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1033,10 +993,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2026-01-13T15:30:47</t>
-        </is>
+      <c r="F18" s="2" t="n">
+        <v>46035.64637731481</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1068,10 +1026,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2026-01-09T08:55:25</t>
-        </is>
+      <c r="F19" s="2" t="n">
+        <v>46031.37181712963</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1103,10 +1059,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2025-11-26T11:14:26</t>
-        </is>
+      <c r="F20" s="2" t="n">
+        <v>45987.46835648148</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1138,10 +1092,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2025-07-31T08:12:37</t>
-        </is>
+      <c r="F21" s="2" t="n">
+        <v>45869.34209490741</v>
       </c>
     </row>
     <row r="22">
@@ -1168,10 +1120,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2025-07-30T17:54:18</t>
-        </is>
+      <c r="F22" s="2" t="n">
+        <v>45868.74604166667</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1203,10 +1153,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2025-09-12T13:16:08</t>
-        </is>
+      <c r="F23" s="2" t="n">
+        <v>45912.55287037037</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1238,10 +1186,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2025-12-16T15:51:12</t>
-        </is>
+      <c r="F24" s="2" t="n">
+        <v>46007.66055555556</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1273,10 +1219,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>2026-02-05T11:35:45</t>
-        </is>
+      <c r="F25" s="2" t="n">
+        <v>46058.48315972222</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1308,10 +1252,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>2026-02-02T09:09:08</t>
-        </is>
+      <c r="F26" s="2" t="n">
+        <v>46055.38134259259</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1343,10 +1285,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>2026-01-15T08:19:46</t>
-        </is>
+      <c r="F27" s="2" t="n">
+        <v>46037.34706018519</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1378,10 +1318,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>2026-02-02T10:50:54</t>
-        </is>
+      <c r="F28" s="2" t="n">
+        <v>46055.45201388889</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1413,10 +1351,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>2025-08-21T10:46:28</t>
-        </is>
+      <c r="F29" s="2" t="n">
+        <v>45890.44893518519</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1448,10 +1384,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>2025-12-31T07:33:04</t>
-        </is>
+      <c r="F30" s="2" t="n">
+        <v>46022.31462962963</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1483,10 +1417,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>2025-08-11T11:47:46</t>
-        </is>
+      <c r="F31" s="2" t="n">
+        <v>45880.49150462963</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1518,10 +1450,8 @@
           <t>Em manutenção</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>2025-10-03T11:32:59</t>
-        </is>
+      <c r="F32" s="2" t="n">
+        <v>45933.48123842593</v>
       </c>
     </row>
     <row r="33">
@@ -1548,10 +1478,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>2026-02-02T15:30:03</t>
-        </is>
+      <c r="F33" s="2" t="n">
+        <v>46055.64586805556</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1583,10 +1511,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>2025-07-31T16:41:24</t>
-        </is>
+      <c r="F34" s="2" t="n">
+        <v>45869.69541666667</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1618,10 +1544,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>2026-02-09T15:05:49</t>
-        </is>
+      <c r="F35" s="2" t="n">
+        <v>46062.62903935185</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1653,10 +1577,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>2025-07-31T12:34:43</t>
-        </is>
+      <c r="F36" s="2" t="n">
+        <v>45869.52410879629</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1688,10 +1610,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>2025-07-31T08:33:04</t>
-        </is>
+      <c r="F37" s="2" t="n">
+        <v>45869.3562962963</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1723,10 +1643,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>2026-02-18T14:47:18</t>
-        </is>
+      <c r="F38" s="2" t="n">
+        <v>46071.61618055555</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1758,10 +1676,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>2025-12-02T09:12:19</t>
-        </is>
+      <c r="F39" s="2" t="n">
+        <v>45993.38355324074</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1793,10 +1709,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>2025-12-22T17:00:01</t>
-        </is>
+      <c r="F40" s="2" t="n">
+        <v>46013.70834490741</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1828,10 +1742,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>2025-08-20T15:57:14</t>
-        </is>
+      <c r="F41" s="2" t="n">
+        <v>45889.66474537037</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1863,10 +1775,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>2026-02-14T23:58:34</t>
-        </is>
+      <c r="F42" s="2" t="n">
+        <v>46067.99900462963</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1898,10 +1808,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>2026-02-11T14:29:21</t>
-        </is>
+      <c r="F43" s="2" t="n">
+        <v>46064.60371527778</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1933,10 +1841,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>2026-01-14T16:52:39</t>
-        </is>
+      <c r="F44" s="2" t="n">
+        <v>46036.70322916667</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1968,10 +1874,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>2025-09-04T14:47:33</t>
-        </is>
+      <c r="F45" s="2" t="n">
+        <v>45904.61635416667</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2003,10 +1907,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>2026-02-05T08:45:14</t>
-        </is>
+      <c r="F46" s="2" t="n">
+        <v>46058.36474537037</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2038,10 +1940,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>2025-10-14T15:43:18</t>
-        </is>
+      <c r="F47" s="2" t="n">
+        <v>45944.65506944444</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2073,10 +1973,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>2025-09-04T14:34:45</t>
-        </is>
+      <c r="F48" s="2" t="n">
+        <v>45904.60746527778</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2108,10 +2006,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>2026-01-08T22:41:31</t>
-        </is>
+      <c r="F49" s="2" t="n">
+        <v>46030.94549768518</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2143,10 +2039,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>2026-02-05T15:09:58</t>
-        </is>
+      <c r="F50" s="2" t="n">
+        <v>46058.6319212963</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2178,10 +2072,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>2025-09-04T09:02:09</t>
-        </is>
+      <c r="F51" s="2" t="n">
+        <v>45904.37649305556</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2213,10 +2105,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>2026-01-29T09:53:30</t>
-        </is>
+      <c r="F52" s="2" t="n">
+        <v>46051.41215277778</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2248,10 +2138,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>2026-01-09T14:59:03</t>
-        </is>
+      <c r="F53" s="2" t="n">
+        <v>46031.62434027778</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2283,10 +2171,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>2026-02-11T10:49:40</t>
-        </is>
+      <c r="F54" s="2" t="n">
+        <v>46064.45115740741</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2318,10 +2204,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>2026-01-22T09:17:12</t>
-        </is>
+      <c r="F55" s="2" t="n">
+        <v>46044.38694444444</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2353,10 +2237,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>2026-01-28T14:41:57</t>
-        </is>
+      <c r="F56" s="2" t="n">
+        <v>46050.61246527778</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2388,10 +2270,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>2026-01-20T10:12:07</t>
-        </is>
+      <c r="F57" s="2" t="n">
+        <v>46042.42508101852</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2423,10 +2303,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>2026-02-11T14:32:29</t>
-        </is>
+      <c r="F58" s="2" t="n">
+        <v>46064.6058912037</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2458,10 +2336,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>2025-09-03T14:25:28</t>
-        </is>
+      <c r="F59" s="2" t="n">
+        <v>45903.60101851852</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2493,10 +2369,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>2026-02-09T07:19:35</t>
-        </is>
+      <c r="F60" s="2" t="n">
+        <v>46062.3052662037</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2528,10 +2402,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>2026-01-23T10:01:22</t>
-        </is>
+      <c r="F61" s="2" t="n">
+        <v>46045.41761574074</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2563,10 +2435,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>2025-09-15T11:12:48</t>
-        </is>
+      <c r="F62" s="2" t="n">
+        <v>45915.46722222222</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2598,10 +2468,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>2025-08-22T11:30:11</t>
-        </is>
+      <c r="F63" s="2" t="n">
+        <v>45891.47929398148</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2633,10 +2501,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>2025-09-04T11:30:32</t>
-        </is>
+      <c r="F64" s="2" t="n">
+        <v>45904.47953703703</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2668,10 +2534,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>2025-09-04T19:41:45</t>
-        </is>
+      <c r="F65" s="2" t="n">
+        <v>45904.82065972222</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2703,10 +2567,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>2025-09-04T11:28:42</t>
-        </is>
+      <c r="F66" s="2" t="n">
+        <v>45904.47826388889</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2738,10 +2600,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>2026-02-10T10:54:58</t>
-        </is>
+      <c r="F67" s="2" t="n">
+        <v>46063.45483796296</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2773,10 +2633,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>2025-12-29T18:02:12</t>
-        </is>
+      <c r="F68" s="2" t="n">
+        <v>46020.75152777778</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2808,10 +2666,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>2026-01-30T14:36:44</t>
-        </is>
+      <c r="F69" s="2" t="n">
+        <v>46052.60884259259</v>
       </c>
     </row>
     <row r="70">
@@ -2838,10 +2694,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>2026-02-02T14:45:30</t>
-        </is>
+      <c r="F70" s="2" t="n">
+        <v>46055.61493055556</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2873,10 +2727,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>2026-01-19T17:05:29</t>
-        </is>
+      <c r="F71" s="2" t="n">
+        <v>46041.7121412037</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2908,10 +2760,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>2026-02-07T11:14:43</t>
-        </is>
+      <c r="F72" s="2" t="n">
+        <v>46060.46855324074</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2943,10 +2793,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:01:13</t>
-        </is>
+      <c r="F73" s="2" t="n">
+        <v>45868.66751157407</v>
       </c>
     </row>
     <row r="74">
@@ -2973,10 +2821,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:36:34</t>
-        </is>
+      <c r="F74" s="2" t="n">
+        <v>45868.69206018518</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3008,10 +2854,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>2026-02-09T15:17:43</t>
-        </is>
+      <c r="F75" s="2" t="n">
+        <v>46062.63730324074</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3043,10 +2887,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>2025-08-26T10:43:33</t>
-        </is>
+      <c r="F76" s="2" t="n">
+        <v>45895.44690972222</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3078,10 +2920,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>2026-02-18T15:00:46</t>
-        </is>
+      <c r="F77" s="2" t="n">
+        <v>46071.62553240741</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3113,10 +2953,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>2025-12-01T08:32:14</t>
-        </is>
+      <c r="F78" s="2" t="n">
+        <v>45992.3557175926</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3148,10 +2986,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>2025-12-17T10:52:03</t>
-        </is>
+      <c r="F79" s="2" t="n">
+        <v>46008.4528125</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3183,10 +3019,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>2025-12-02T21:41:15</t>
-        </is>
+      <c r="F80" s="2" t="n">
+        <v>45993.90364583334</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3218,10 +3052,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>2025-12-02T08:50:09</t>
-        </is>
+      <c r="F81" s="2" t="n">
+        <v>45993.36815972222</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -3253,10 +3085,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>2025-11-26T17:20:52</t>
-        </is>
+      <c r="F82" s="2" t="n">
+        <v>45987.72282407407</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3288,10 +3118,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>2026-01-20T14:20:49</t>
-        </is>
+      <c r="F83" s="2" t="n">
+        <v>46042.59778935185</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3323,10 +3151,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>2026-02-02T15:26:51</t>
-        </is>
+      <c r="F84" s="2" t="n">
+        <v>46055.64364583333</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3358,10 +3184,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>2026-02-06T14:18:39</t>
-        </is>
+      <c r="F85" s="2" t="n">
+        <v>46059.59628472223</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3393,10 +3217,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>2026-01-23T08:20:09</t>
-        </is>
+      <c r="F86" s="2" t="n">
+        <v>46045.34732638889</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3428,10 +3250,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>2026-02-14T13:56:54</t>
-        </is>
+      <c r="F87" s="2" t="n">
+        <v>46067.58118055556</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3463,10 +3283,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>2026-02-07T08:34:20</t>
-        </is>
+      <c r="F88" s="2" t="n">
+        <v>46060.35717592593</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3498,10 +3316,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>2025-07-31T15:30:16</t>
-        </is>
+      <c r="F89" s="2" t="n">
+        <v>45869.64601851852</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3533,10 +3349,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>2026-02-20T09:27:01</t>
-        </is>
+      <c r="F90" s="2" t="n">
+        <v>46073.39376157407</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -3568,10 +3382,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>2026-02-12T14:45:40</t>
-        </is>
+      <c r="F91" s="2" t="n">
+        <v>46065.6150462963</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3603,10 +3415,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>2025-12-22T15:48:11</t>
-        </is>
+      <c r="F92" s="2" t="n">
+        <v>46013.65846064815</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3638,10 +3448,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>2026-02-02T17:17:07</t>
-        </is>
+      <c r="F93" s="2" t="n">
+        <v>46055.72021990741</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3673,10 +3481,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>2025-07-31T09:13:59</t>
-        </is>
+      <c r="F94" s="2" t="n">
+        <v>45869.38471064815</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -3708,10 +3514,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>2026-02-06T16:19:39</t>
-        </is>
+      <c r="F95" s="2" t="n">
+        <v>46059.6803125</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3743,10 +3547,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>2026-01-05T12:06:27</t>
-        </is>
+      <c r="F96" s="2" t="n">
+        <v>46027.50447916667</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -3778,10 +3580,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>2025-12-22T16:53:21</t>
-        </is>
+      <c r="F97" s="2" t="n">
+        <v>46013.70371527778</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3813,10 +3613,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>2026-02-19T16:46:46</t>
-        </is>
+      <c r="F98" s="2" t="n">
+        <v>46072.69914351852</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3848,10 +3646,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>2026-01-20T11:33:21</t>
-        </is>
+      <c r="F99" s="2" t="n">
+        <v>46042.48149305556</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -3883,10 +3679,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>2026-02-19T09:34:36</t>
-        </is>
+      <c r="F100" s="2" t="n">
+        <v>46072.39902777778</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -3918,10 +3712,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>2025-10-15T19:57:50</t>
-        </is>
+      <c r="F101" s="2" t="n">
+        <v>45945.8318287037</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3953,10 +3745,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>2025-09-03T09:54:33</t>
-        </is>
+      <c r="F102" s="2" t="n">
+        <v>45903.41288194444</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -3988,10 +3778,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>2025-10-15T19:57:50</t>
-        </is>
+      <c r="F103" s="2" t="n">
+        <v>45945.8318287037</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4023,10 +3811,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>2026-02-04T22:17:25</t>
-        </is>
+      <c r="F104" s="2" t="n">
+        <v>46057.92876157408</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4058,10 +3844,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>2025-09-10T09:11:03</t>
-        </is>
+      <c r="F105" s="2" t="n">
+        <v>45910.38267361111</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4093,10 +3877,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>2025-08-22T09:07:52</t>
-        </is>
+      <c r="F106" s="2" t="n">
+        <v>45891.38046296296</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4128,10 +3910,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>2025-08-28T15:51:54</t>
-        </is>
+      <c r="F107" s="2" t="n">
+        <v>45897.66104166667</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
@@ -4163,10 +3943,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>2026-02-11T09:59:15</t>
-        </is>
+      <c r="F108" s="2" t="n">
+        <v>46064.41614583333</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
@@ -4198,10 +3976,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:46:00</t>
-        </is>
+      <c r="F109" s="2" t="n">
+        <v>45868.65694444445</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
@@ -4233,10 +4009,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:20:14</t>
-        </is>
+      <c r="F110" s="2" t="n">
+        <v>45868.63905092593</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4268,10 +4042,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>2025-11-22T08:19:27</t>
-        </is>
+      <c r="F111" s="2" t="n">
+        <v>45983.34684027778</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4303,10 +4075,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>2025-11-19T16:24:07</t>
-        </is>
+      <c r="F112" s="2" t="n">
+        <v>45980.68341435185</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4338,10 +4108,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>2025-07-31T10:57:15</t>
-        </is>
+      <c r="F113" s="2" t="n">
+        <v>45869.45642361111</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4373,10 +4141,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:12:40</t>
-        </is>
+      <c r="F114" s="2" t="n">
+        <v>45868.67546296296</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -4408,10 +4174,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>2025-07-30T19:05:34</t>
-        </is>
+      <c r="F115" s="2" t="n">
+        <v>45868.79553240741</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4443,10 +4207,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>2025-07-31T16:03:01</t>
-        </is>
+      <c r="F116" s="2" t="n">
+        <v>45869.66876157407</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -4478,10 +4240,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>2026-02-19T09:28:44</t>
-        </is>
+      <c r="F117" s="2" t="n">
+        <v>46072.3949537037</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -4513,10 +4273,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>2025-07-31T19:18:50</t>
-        </is>
+      <c r="F118" s="2" t="n">
+        <v>45869.80474537037</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -4548,10 +4306,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>2025-09-01T07:28:13</t>
-        </is>
+      <c r="F119" s="2" t="n">
+        <v>45901.31126157408</v>
       </c>
     </row>
     <row r="120">
@@ -4578,10 +4334,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>2025-09-15T07:44:36</t>
-        </is>
+      <c r="F120" s="2" t="n">
+        <v>45915.32263888889</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4613,10 +4367,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>2026-01-12T08:24:00</t>
-        </is>
+      <c r="F121" s="2" t="n">
+        <v>46034.35</v>
       </c>
     </row>
     <row r="122">
@@ -4643,10 +4395,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>2026-02-18T08:58:09</t>
-        </is>
+      <c r="F122" s="2" t="n">
+        <v>46071.37371527778</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -4678,10 +4428,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>2026-02-18T12:47:20</t>
-        </is>
+      <c r="F123" s="2" t="n">
+        <v>46071.53287037037</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -4713,10 +4461,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>2026-02-19T09:03:30</t>
-        </is>
+      <c r="F124" s="2" t="n">
+        <v>46072.37743055556</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -4748,10 +4494,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>2025-09-15T07:44:36</t>
-        </is>
+      <c r="F125" s="2" t="n">
+        <v>45915.32263888889</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -4783,10 +4527,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>2026-02-02T07:40:44</t>
-        </is>
+      <c r="F126" s="2" t="n">
+        <v>46055.31995370371</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -4818,10 +4560,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>2026-02-18T08:58:09</t>
-        </is>
+      <c r="F127" s="2" t="n">
+        <v>46071.37371527778</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -4853,10 +4593,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>2026-02-18T12:47:20</t>
-        </is>
+      <c r="F128" s="2" t="n">
+        <v>46071.53287037037</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -4888,10 +4626,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:05:32</t>
-        </is>
+      <c r="F129" s="2" t="n">
+        <v>45868.67050925926</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -4923,10 +4659,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>2026-02-19T13:10:57</t>
-        </is>
+      <c r="F130" s="2" t="n">
+        <v>46072.54927083333</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -4958,10 +4692,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>2026-02-19T06:51:08</t>
-        </is>
+      <c r="F131" s="2" t="n">
+        <v>46072.28550925926</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
@@ -4993,10 +4725,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>2026-02-18T07:52:17</t>
-        </is>
+      <c r="F132" s="2" t="n">
+        <v>46071.32797453704</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
@@ -5028,10 +4758,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>2026-02-09T09:22:20</t>
-        </is>
+      <c r="F133" s="2" t="n">
+        <v>46062.39050925926</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -5063,10 +4791,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>2026-02-19T13:10:57</t>
-        </is>
+      <c r="F134" s="2" t="n">
+        <v>46072.54927083333</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -5098,10 +4824,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>2026-01-24T09:13:07</t>
-        </is>
+      <c r="F135" s="2" t="n">
+        <v>46046.38410879629</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -5133,10 +4857,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>2026-02-19T09:03:30</t>
-        </is>
+      <c r="F136" s="2" t="n">
+        <v>46072.37743055556</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -5168,10 +4890,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>2026-02-19T06:51:08</t>
-        </is>
+      <c r="F137" s="2" t="n">
+        <v>46072.28550925926</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -5203,10 +4923,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>2025-12-08T08:49:27</t>
-        </is>
+      <c r="F138" s="2" t="n">
+        <v>45999.36767361111</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -5238,10 +4956,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>2025-11-06T17:06:12</t>
-        </is>
+      <c r="F139" s="2" t="n">
+        <v>45967.71263888889</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -5273,10 +4989,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>2025-07-31T19:21:17</t>
-        </is>
+      <c r="F140" s="2" t="n">
+        <v>45869.80644675926</v>
       </c>
     </row>
     <row r="141">
@@ -5303,10 +5017,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>2026-01-16T09:05:12</t>
-        </is>
+      <c r="F141" s="2" t="n">
+        <v>46038.37861111111</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -5338,10 +5050,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>2026-02-05T08:31:46</t>
-        </is>
+      <c r="F142" s="2" t="n">
+        <v>46058.35539351852</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -5373,10 +5083,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>2026-02-03T14:49:32</t>
-        </is>
+      <c r="F143" s="2" t="n">
+        <v>46056.61773148148</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -5408,10 +5116,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>2026-02-19T07:54:27</t>
-        </is>
+      <c r="F144" s="2" t="n">
+        <v>46072.32947916666</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -5443,10 +5149,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:34:41</t>
-        </is>
+      <c r="F145" s="2" t="n">
+        <v>45868.64908564815</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -5478,10 +5182,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>2026-02-04T10:07:26</t>
-        </is>
+      <c r="F146" s="2" t="n">
+        <v>46057.4218287037</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
@@ -5513,10 +5215,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>2026-01-13T15:34:44</t>
-        </is>
+      <c r="F147" s="2" t="n">
+        <v>46035.64912037037</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -5548,10 +5248,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>2025-11-14T14:46:29</t>
-        </is>
+      <c r="F148" s="2" t="n">
+        <v>45975.61561342593</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -5583,10 +5281,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>2026-02-19T13:37:04</t>
-        </is>
+      <c r="F149" s="2" t="n">
+        <v>46072.5674074074</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -5618,10 +5314,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>2025-07-31T11:39:50</t>
-        </is>
+      <c r="F150" s="2" t="n">
+        <v>45869.48599537037</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -5653,10 +5347,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>2025-08-04T12:55:52</t>
-        </is>
+      <c r="F151" s="2" t="n">
+        <v>45873.5387962963</v>
       </c>
     </row>
     <row r="152">
@@ -5683,10 +5375,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F152" t="inlineStr">
-        <is>
-          <t>2026-02-04T13:11:56</t>
-        </is>
+      <c r="F152" s="2" t="n">
+        <v>46057.5499537037</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -5718,10 +5408,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F153" t="inlineStr">
-        <is>
-          <t>2026-02-19T22:24:45</t>
-        </is>
+      <c r="F153" s="2" t="n">
+        <v>46072.93385416667</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -5753,10 +5441,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>2025-12-29T09:49:40</t>
-        </is>
+      <c r="F154" s="2" t="n">
+        <v>46020.40949074074</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -5788,10 +5474,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>2026-02-19T08:02:06</t>
-        </is>
+      <c r="F155" s="2" t="n">
+        <v>46072.33479166667</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
@@ -5823,10 +5507,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F156" t="inlineStr">
-        <is>
-          <t>2026-02-02T18:16:08</t>
-        </is>
+      <c r="F156" s="2" t="n">
+        <v>46055.7612037037</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
@@ -5858,10 +5540,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t>2025-08-01T10:01:54</t>
-        </is>
+      <c r="F157" s="2" t="n">
+        <v>45870.41798611111</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
@@ -5893,10 +5573,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>2025-11-18T13:58:40</t>
-        </is>
+      <c r="F158" s="2" t="n">
+        <v>45979.5824074074</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -5928,10 +5606,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F159" t="inlineStr">
-        <is>
-          <t>2025-07-31T06:46:34</t>
-        </is>
+      <c r="F159" s="2" t="n">
+        <v>45869.28233796296</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -5963,10 +5639,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>2025-07-30T18:35:43</t>
-        </is>
+      <c r="F160" s="2" t="n">
+        <v>45868.77480324074</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -5998,10 +5672,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F161" t="inlineStr">
-        <is>
-          <t>2026-02-20T09:30:21</t>
-        </is>
+      <c r="F161" s="2" t="n">
+        <v>46073.39607638889</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -6033,10 +5705,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t>2025-09-04T11:11:16</t>
-        </is>
+      <c r="F162" s="2" t="n">
+        <v>45904.46615740741</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -6068,10 +5738,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:46:47</t>
-        </is>
+      <c r="F163" s="2" t="n">
+        <v>45868.65748842592</v>
       </c>
     </row>
     <row r="164">
@@ -6098,10 +5766,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F164" t="inlineStr">
-        <is>
-          <t>2025-12-31T11:19:54</t>
-        </is>
+      <c r="F164" s="2" t="n">
+        <v>46022.47215277778</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -6133,10 +5799,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F165" t="inlineStr">
-        <is>
-          <t>2025-11-21T15:31:11</t>
-        </is>
+      <c r="F165" s="2" t="n">
+        <v>45982.64665509259</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -6168,10 +5832,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F166" t="inlineStr">
-        <is>
-          <t>2026-02-12T16:16:03</t>
-        </is>
+      <c r="F166" s="2" t="n">
+        <v>46065.6778125</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -6203,10 +5865,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F167" t="inlineStr">
-        <is>
-          <t>2026-02-19T14:55:42</t>
-        </is>
+      <c r="F167" s="2" t="n">
+        <v>46072.62201388889</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -6238,10 +5898,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>2026-02-14T16:23:01</t>
-        </is>
+      <c r="F168" s="2" t="n">
+        <v>46067.68265046296</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -6273,10 +5931,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F169" t="inlineStr">
-        <is>
-          <t>2026-01-31T08:06:24</t>
-        </is>
+      <c r="F169" s="2" t="n">
+        <v>46053.33777777778</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -6308,10 +5964,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F170" t="inlineStr">
-        <is>
-          <t>2025-08-04T08:52:38</t>
-        </is>
+      <c r="F170" s="2" t="n">
+        <v>45873.36988425926</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -6343,10 +5997,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F171" t="inlineStr">
-        <is>
-          <t>2025-07-31T02:24:14</t>
-        </is>
+      <c r="F171" s="2" t="n">
+        <v>45869.10016203704</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -6378,10 +6030,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F172" t="inlineStr">
-        <is>
-          <t>2026-02-02T20:08:57</t>
-        </is>
+      <c r="F172" s="2" t="n">
+        <v>46055.83954861111</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -6413,10 +6063,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F173" t="inlineStr">
-        <is>
-          <t>2026-02-11T10:28:00</t>
-        </is>
+      <c r="F173" s="2" t="n">
+        <v>46064.43611111111</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -6448,10 +6096,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F174" t="inlineStr">
-        <is>
-          <t>2026-01-30T12:47:02</t>
-        </is>
+      <c r="F174" s="2" t="n">
+        <v>46052.53266203704</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -6483,10 +6129,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F175" t="inlineStr">
-        <is>
-          <t>2025-07-30T17:54:18</t>
-        </is>
+      <c r="F175" s="2" t="n">
+        <v>45868.74604166667</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6518,10 +6162,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F176" t="inlineStr">
-        <is>
-          <t>2026-02-10T14:14:45</t>
-        </is>
+      <c r="F176" s="2" t="n">
+        <v>46063.59357638889</v>
       </c>
     </row>
     <row r="177">
@@ -6548,10 +6190,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F177" t="inlineStr">
-        <is>
-          <t>2025-07-31T02:24:14</t>
-        </is>
+      <c r="F177" s="2" t="n">
+        <v>45869.10016203704</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -6583,10 +6223,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr">
-        <is>
-          <t>2025-12-22T15:05:52</t>
-        </is>
+      <c r="F178" s="2" t="n">
+        <v>46013.62907407407</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -6618,10 +6256,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr">
-        <is>
-          <t>2026-02-04T14:35:02</t>
-        </is>
+      <c r="F179" s="2" t="n">
+        <v>46057.60766203704</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -6653,10 +6289,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr">
-        <is>
-          <t>2026-02-19T23:41:47</t>
-        </is>
+      <c r="F180" s="2" t="n">
+        <v>46072.98734953703</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -6688,10 +6322,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr">
-        <is>
-          <t>2026-02-19T14:03:00</t>
-        </is>
+      <c r="F181" s="2" t="n">
+        <v>46072.58541666667</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -6723,10 +6355,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr">
-        <is>
-          <t>2025-12-22T10:56:15</t>
-        </is>
+      <c r="F182" s="2" t="n">
+        <v>46013.45572916666</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -6758,10 +6388,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr">
-        <is>
-          <t>2025-07-31T08:30:53</t>
-        </is>
+      <c r="F183" s="2" t="n">
+        <v>45869.3547800926</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -6793,10 +6421,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F184" t="inlineStr">
-        <is>
-          <t>2026-02-19T21:27:25</t>
-        </is>
+      <c r="F184" s="2" t="n">
+        <v>46072.89403935185</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -6828,10 +6454,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr">
-        <is>
-          <t>2025-11-06T16:18:42</t>
-        </is>
+      <c r="F185" s="2" t="n">
+        <v>45967.67965277778</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -6863,10 +6487,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F186" t="inlineStr">
-        <is>
-          <t>2025-11-06T17:06:12</t>
-        </is>
+      <c r="F186" s="2" t="n">
+        <v>45967.71263888889</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -6898,10 +6520,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F187" t="inlineStr">
-        <is>
-          <t>2025-11-06T16:46:26</t>
-        </is>
+      <c r="F187" s="2" t="n">
+        <v>45967.69891203703</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -6933,10 +6553,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F188" t="inlineStr">
-        <is>
-          <t>2026-02-02T17:17:07</t>
-        </is>
+      <c r="F188" s="2" t="n">
+        <v>46055.72021990741</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -6968,10 +6586,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F189" t="inlineStr">
-        <is>
-          <t>2025-07-30T18:36:11</t>
-        </is>
+      <c r="F189" s="2" t="n">
+        <v>45868.77512731482</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -7003,10 +6619,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F190" t="inlineStr">
-        <is>
-          <t>2026-02-11T09:59:15</t>
-        </is>
+      <c r="F190" s="2" t="n">
+        <v>46064.41614583333</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -7038,10 +6652,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F191" t="inlineStr">
-        <is>
-          <t>2025-11-17T08:18:59</t>
-        </is>
+      <c r="F191" s="2" t="n">
+        <v>45978.3465162037</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -7073,10 +6685,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F192" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:50:40</t>
-        </is>
+      <c r="F192" s="2" t="n">
+        <v>45868.66018518519</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -7108,10 +6718,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F193" t="inlineStr">
-        <is>
-          <t>2026-02-11T14:37:47</t>
-        </is>
+      <c r="F193" s="2" t="n">
+        <v>46064.60957175926</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -7143,10 +6751,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F194" t="inlineStr">
-        <is>
-          <t>2026-02-04T22:17:25</t>
-        </is>
+      <c r="F194" s="2" t="n">
+        <v>46057.92876157408</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
@@ -7178,10 +6784,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F195" t="inlineStr">
-        <is>
-          <t>2026-02-13T08:14:44</t>
-        </is>
+      <c r="F195" s="2" t="n">
+        <v>46066.34356481482</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
@@ -7213,10 +6817,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F196" t="inlineStr">
-        <is>
-          <t>2026-02-09T23:58:37</t>
-        </is>
+      <c r="F196" s="2" t="n">
+        <v>46062.99903935185</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
@@ -7248,10 +6850,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr">
-        <is>
-          <t>2026-01-14T18:36:44</t>
-        </is>
+      <c r="F197" s="2" t="n">
+        <v>46036.77550925926</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
@@ -7283,10 +6883,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F198" t="inlineStr">
-        <is>
-          <t>2026-01-08T08:43:45</t>
-        </is>
+      <c r="F198" s="2" t="n">
+        <v>46030.36371527778</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
@@ -7318,10 +6916,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F199" t="inlineStr">
-        <is>
-          <t>2025-12-23T07:31:43</t>
-        </is>
+      <c r="F199" s="2" t="n">
+        <v>46014.31369212963</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -7353,10 +6949,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F200" t="inlineStr">
-        <is>
-          <t>2025-07-30T19:47:32</t>
-        </is>
+      <c r="F200" s="2" t="n">
+        <v>45868.82467592593</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
@@ -7388,10 +6982,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F201" t="inlineStr">
-        <is>
-          <t>2025-07-30T17:42:47</t>
-        </is>
+      <c r="F201" s="2" t="n">
+        <v>45868.73804398148</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -7423,10 +7015,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F202" t="inlineStr">
-        <is>
-          <t>2026-02-19T15:38:57</t>
-        </is>
+      <c r="F202" s="2" t="n">
+        <v>46072.65204861111</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -7458,10 +7048,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F203" t="inlineStr">
-        <is>
-          <t>2026-02-19T15:35:26</t>
-        </is>
+      <c r="F203" s="2" t="n">
+        <v>46072.64960648148</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -7493,10 +7081,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F204" t="inlineStr">
-        <is>
-          <t>2026-02-12T14:44:53</t>
-        </is>
+      <c r="F204" s="2" t="n">
+        <v>46065.61450231481</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -7528,10 +7114,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F205" t="inlineStr">
-        <is>
-          <t>2025-12-31T13:57:29</t>
-        </is>
+      <c r="F205" s="2" t="n">
+        <v>46022.58158564815</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
@@ -7563,10 +7147,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F206" t="inlineStr">
-        <is>
-          <t>2026-02-03T16:11:26</t>
-        </is>
+      <c r="F206" s="2" t="n">
+        <v>46056.67460648148</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -7598,10 +7180,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F207" t="inlineStr">
-        <is>
-          <t>2025-07-31T07:41:44</t>
-        </is>
+      <c r="F207" s="2" t="n">
+        <v>45869.32064814815</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -7633,10 +7213,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F208" t="inlineStr">
-        <is>
-          <t>2025-07-31T08:39:29</t>
-        </is>
+      <c r="F208" s="2" t="n">
+        <v>45869.36075231482</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -7668,10 +7246,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F209" t="inlineStr">
-        <is>
-          <t>2025-08-11T09:36:33</t>
-        </is>
+      <c r="F209" s="2" t="n">
+        <v>45880.40038194445</v>
       </c>
       <c r="G209" t="inlineStr">
         <is>
@@ -7703,10 +7279,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F210" t="inlineStr">
-        <is>
-          <t>2026-01-22T09:17:12</t>
-        </is>
+      <c r="F210" s="2" t="n">
+        <v>46044.38694444444</v>
       </c>
       <c r="G210" t="inlineStr">
         <is>
@@ -7738,10 +7312,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F211" t="inlineStr">
-        <is>
-          <t>2025-07-31T07:44:41</t>
-        </is>
+      <c r="F211" s="2" t="n">
+        <v>45869.32269675926</v>
       </c>
       <c r="G211" t="inlineStr">
         <is>
@@ -7773,10 +7345,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F212" t="inlineStr">
-        <is>
-          <t>2025-10-14T10:08:10</t>
-        </is>
+      <c r="F212" s="2" t="n">
+        <v>45944.42233796296</v>
       </c>
       <c r="G212" t="inlineStr">
         <is>
@@ -7808,10 +7378,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F213" t="inlineStr">
-        <is>
-          <t>2025-07-31T12:15:19</t>
-        </is>
+      <c r="F213" s="2" t="n">
+        <v>45869.51063657407</v>
       </c>
       <c r="G213" t="inlineStr">
         <is>
@@ -7843,10 +7411,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F214" t="inlineStr">
-        <is>
-          <t>2025-11-10T08:18:12</t>
-        </is>
+      <c r="F214" s="2" t="n">
+        <v>45971.34597222223</v>
       </c>
     </row>
     <row r="215">
@@ -7873,10 +7439,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F215" t="inlineStr">
-        <is>
-          <t>2026-02-09T23:58:37</t>
-        </is>
+      <c r="F215" s="2" t="n">
+        <v>46062.99903935185</v>
       </c>
       <c r="G215" t="inlineStr">
         <is>
@@ -7908,10 +7472,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F216" t="inlineStr">
-        <is>
-          <t>2025-11-19T04:58:01</t>
-        </is>
+      <c r="F216" s="2" t="n">
+        <v>45980.20695601852</v>
       </c>
       <c r="G216" t="inlineStr">
         <is>
@@ -7943,10 +7505,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F217" t="inlineStr">
-        <is>
-          <t>2026-01-26T08:06:56</t>
-        </is>
+      <c r="F217" s="2" t="n">
+        <v>46048.33814814815</v>
       </c>
       <c r="G217" t="inlineStr">
         <is>
@@ -7978,10 +7538,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F218" t="inlineStr">
-        <is>
-          <t>2025-12-22T19:40:50</t>
-        </is>
+      <c r="F218" s="2" t="n">
+        <v>46013.82002314815</v>
       </c>
       <c r="G218" t="inlineStr">
         <is>
@@ -8013,10 +7571,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F219" t="inlineStr">
-        <is>
-          <t>2026-01-09T14:08:22</t>
-        </is>
+      <c r="F219" s="2" t="n">
+        <v>46031.58914351852</v>
       </c>
       <c r="G219" t="inlineStr">
         <is>
@@ -8048,10 +7604,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F220" t="inlineStr">
-        <is>
-          <t>2026-01-30T14:46:26</t>
-        </is>
+      <c r="F220" s="2" t="n">
+        <v>46052.61557870371</v>
       </c>
       <c r="G220" t="inlineStr">
         <is>
@@ -8083,10 +7637,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F221" t="inlineStr">
-        <is>
-          <t>2026-01-09T14:08:29</t>
-        </is>
+      <c r="F221" s="2" t="n">
+        <v>46031.58922453703</v>
       </c>
       <c r="G221" t="inlineStr">
         <is>
@@ -8118,10 +7670,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F222" t="inlineStr">
-        <is>
-          <t>2026-02-02T20:08:57</t>
-        </is>
+      <c r="F222" s="2" t="n">
+        <v>46055.83954861111</v>
       </c>
       <c r="G222" t="inlineStr">
         <is>
@@ -8153,10 +7703,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F223" t="inlineStr">
-        <is>
-          <t>2026-02-13T11:52:22</t>
-        </is>
+      <c r="F223" s="2" t="n">
+        <v>46066.49469907407</v>
       </c>
       <c r="G223" t="inlineStr">
         <is>
@@ -8188,10 +7736,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F224" t="inlineStr">
-        <is>
-          <t>2025-07-31T07:41:44</t>
-        </is>
+      <c r="F224" s="2" t="n">
+        <v>45869.32064814815</v>
       </c>
       <c r="G224" t="inlineStr">
         <is>
@@ -8223,10 +7769,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F225" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:43:03</t>
-        </is>
+      <c r="F225" s="2" t="n">
+        <v>45868.6965625</v>
       </c>
       <c r="G225" t="inlineStr">
         <is>
@@ -8258,10 +7802,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F226" t="inlineStr">
-        <is>
-          <t>2026-01-21T10:09:35</t>
-        </is>
+      <c r="F226" s="2" t="n">
+        <v>46043.42332175926</v>
       </c>
       <c r="G226" t="inlineStr">
         <is>
@@ -8293,10 +7835,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F227" t="inlineStr">
-        <is>
-          <t>2026-01-23T10:01:22</t>
-        </is>
+      <c r="F227" s="2" t="n">
+        <v>46045.41761574074</v>
       </c>
       <c r="G227" t="inlineStr">
         <is>
@@ -8328,10 +7868,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F228" t="inlineStr">
-        <is>
-          <t>2025-12-09T10:07:15</t>
-        </is>
+      <c r="F228" s="2" t="n">
+        <v>46000.42170138889</v>
       </c>
       <c r="G228" t="inlineStr">
         <is>
@@ -8363,10 +7901,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F229" t="inlineStr">
-        <is>
-          <t>2026-01-29T14:39:22</t>
-        </is>
+      <c r="F229" s="2" t="n">
+        <v>46051.61067129629</v>
       </c>
       <c r="G229" t="inlineStr">
         <is>
@@ -8398,10 +7934,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F230" t="inlineStr">
-        <is>
-          <t>2026-01-06T10:16:57</t>
-        </is>
+      <c r="F230" s="2" t="n">
+        <v>46028.4284375</v>
       </c>
     </row>
     <row r="231">
@@ -8428,10 +7962,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F231" t="inlineStr">
-        <is>
-          <t>2026-01-14T09:51:25</t>
-        </is>
+      <c r="F231" s="2" t="n">
+        <v>46036.41070601852</v>
       </c>
       <c r="G231" t="inlineStr">
         <is>
@@ -8463,10 +7995,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F232" t="inlineStr">
-        <is>
-          <t>2026-01-30T14:36:44</t>
-        </is>
+      <c r="F232" s="2" t="n">
+        <v>46052.60884259259</v>
       </c>
     </row>
     <row r="233">
@@ -8493,10 +8023,8 @@
           <t>Em manutenção</t>
         </is>
       </c>
-      <c r="F233" t="inlineStr">
-        <is>
-          <t>2025-10-03T11:24:55</t>
-        </is>
+      <c r="F233" s="2" t="n">
+        <v>45933.47563657408</v>
       </c>
     </row>
     <row r="234">
@@ -8523,10 +8051,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F234" t="inlineStr">
-        <is>
-          <t>2025-11-21T07:52:34</t>
-        </is>
+      <c r="F234" s="2" t="n">
+        <v>45982.3281712963</v>
       </c>
       <c r="G234" t="inlineStr">
         <is>
@@ -8558,10 +8084,8 @@
           <t>Em manutenção</t>
         </is>
       </c>
-      <c r="F235" t="inlineStr">
-        <is>
-          <t>2025-10-03T11:36:28</t>
-        </is>
+      <c r="F235" s="2" t="n">
+        <v>45933.48365740741</v>
       </c>
     </row>
     <row r="236">
@@ -8588,10 +8112,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F236" t="inlineStr">
-        <is>
-          <t>2026-01-14T14:54:21</t>
-        </is>
+      <c r="F236" s="2" t="n">
+        <v>46036.62107638889</v>
       </c>
     </row>
     <row r="237">
@@ -8618,10 +8140,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F237" t="inlineStr">
-        <is>
-          <t>2026-01-08T13:11:27</t>
-        </is>
+      <c r="F237" s="2" t="n">
+        <v>46030.54961805556</v>
       </c>
     </row>
     <row r="238">
@@ -8648,10 +8168,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F238" t="inlineStr">
-        <is>
-          <t>2026-02-13T08:24:38</t>
-        </is>
+      <c r="F238" s="2" t="n">
+        <v>46066.35043981481</v>
       </c>
       <c r="G238" t="inlineStr">
         <is>
@@ -8683,10 +8201,8 @@
           <t>Em manutenção</t>
         </is>
       </c>
-      <c r="F239" t="inlineStr">
-        <is>
-          <t>2025-10-03T11:31:37</t>
-        </is>
+      <c r="F239" s="2" t="n">
+        <v>45933.48028935185</v>
       </c>
     </row>
     <row r="240">
@@ -8713,10 +8229,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F240" t="inlineStr">
-        <is>
-          <t>2025-10-14T20:39:07</t>
-        </is>
+      <c r="F240" s="2" t="n">
+        <v>45944.86049768519</v>
       </c>
       <c r="G240" t="inlineStr">
         <is>
@@ -8748,10 +8262,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F241" t="inlineStr">
-        <is>
-          <t>2026-01-30T14:36:44</t>
-        </is>
+      <c r="F241" s="2" t="n">
+        <v>46052.60884259259</v>
       </c>
       <c r="G241" t="inlineStr">
         <is>
@@ -8783,10 +8295,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr">
-        <is>
-          <t>2026-02-10T12:58:44</t>
-        </is>
+      <c r="F242" s="2" t="n">
+        <v>46063.54078703704</v>
       </c>
       <c r="G242" t="inlineStr">
         <is>
@@ -8818,10 +8328,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F243" t="inlineStr">
-        <is>
-          <t>2025-12-31T11:15:57</t>
-        </is>
+      <c r="F243" s="2" t="n">
+        <v>46022.46940972222</v>
       </c>
       <c r="G243" t="inlineStr">
         <is>
@@ -8853,10 +8361,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F244" t="inlineStr">
-        <is>
-          <t>2025-08-05T17:51:21</t>
-        </is>
+      <c r="F244" s="2" t="n">
+        <v>45874.74399305556</v>
       </c>
       <c r="G244" t="inlineStr">
         <is>
@@ -8888,10 +8394,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F245" t="inlineStr">
-        <is>
-          <t>2025-08-21T15:00:54</t>
-        </is>
+      <c r="F245" s="2" t="n">
+        <v>45890.625625</v>
       </c>
       <c r="G245" t="inlineStr">
         <is>
@@ -8923,10 +8427,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F246" t="inlineStr">
-        <is>
-          <t>2026-01-29T14:23:54</t>
-        </is>
+      <c r="F246" s="2" t="n">
+        <v>46051.59993055555</v>
       </c>
       <c r="G246" t="inlineStr">
         <is>
@@ -8958,10 +8460,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F247" t="inlineStr">
-        <is>
-          <t>2025-10-02T18:08:01</t>
-        </is>
+      <c r="F247" s="2" t="n">
+        <v>45932.75556712963</v>
       </c>
       <c r="G247" t="inlineStr">
         <is>
@@ -8993,10 +8493,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F248" t="inlineStr">
-        <is>
-          <t>2025-08-01T11:55:28</t>
-        </is>
+      <c r="F248" s="2" t="n">
+        <v>45870.49685185185</v>
       </c>
       <c r="G248" t="inlineStr">
         <is>
@@ -9028,10 +8526,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F249" t="inlineStr">
-        <is>
-          <t>2025-09-08T11:00:05</t>
-        </is>
+      <c r="F249" s="2" t="n">
+        <v>45908.45839120371</v>
       </c>
       <c r="G249" t="inlineStr">
         <is>
@@ -9063,10 +8559,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F250" t="inlineStr">
-        <is>
-          <t>2025-09-04T09:00:24</t>
-        </is>
+      <c r="F250" s="2" t="n">
+        <v>45904.37527777778</v>
       </c>
       <c r="G250" t="inlineStr">
         <is>
@@ -9098,10 +8592,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F251" t="inlineStr">
-        <is>
-          <t>2025-12-31T13:57:29</t>
-        </is>
+      <c r="F251" s="2" t="n">
+        <v>46022.58158564815</v>
       </c>
     </row>
     <row r="252">
@@ -9128,10 +8620,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F252" t="inlineStr">
-        <is>
-          <t>2026-02-03T16:11:26</t>
-        </is>
+      <c r="F252" s="2" t="n">
+        <v>46056.67460648148</v>
       </c>
     </row>
     <row r="253">
@@ -9158,10 +8648,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F253" t="inlineStr">
-        <is>
-          <t>2025-08-09T12:00:19</t>
-        </is>
+      <c r="F253" s="2" t="n">
+        <v>45878.50021990741</v>
       </c>
     </row>
     <row r="254">
@@ -9188,10 +8676,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F254" t="inlineStr">
-        <is>
-          <t>2025-07-31T14:56:32</t>
-        </is>
+      <c r="F254" s="2" t="n">
+        <v>45869.62259259259</v>
       </c>
     </row>
     <row r="255">
@@ -9218,10 +8704,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F255" t="inlineStr">
-        <is>
-          <t>2026-02-20T08:54:23</t>
-        </is>
+      <c r="F255" s="2" t="n">
+        <v>46073.37109953703</v>
       </c>
       <c r="G255" t="inlineStr">
         <is>
@@ -9253,10 +8737,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F256" t="inlineStr">
-        <is>
-          <t>2025-12-09T07:50:04</t>
-        </is>
+      <c r="F256" s="2" t="n">
+        <v>46000.32643518518</v>
       </c>
     </row>
     <row r="257">
@@ -9283,10 +8765,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F257" t="inlineStr">
-        <is>
-          <t>2026-02-14T16:23:01</t>
-        </is>
+      <c r="F257" s="2" t="n">
+        <v>46067.68265046296</v>
       </c>
       <c r="G257" t="inlineStr">
         <is>
@@ -9318,10 +8798,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F258" t="inlineStr">
-        <is>
-          <t>2025-07-31T06:59:23</t>
-        </is>
+      <c r="F258" s="2" t="n">
+        <v>45869.29123842593</v>
       </c>
       <c r="G258" t="inlineStr">
         <is>
@@ -9353,10 +8831,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F259" t="inlineStr">
-        <is>
-          <t>2025-10-05T06:15:38</t>
-        </is>
+      <c r="F259" s="2" t="n">
+        <v>45935.26085648148</v>
       </c>
       <c r="G259" t="inlineStr">
         <is>
@@ -9388,10 +8864,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F260" t="inlineStr">
-        <is>
-          <t>2025-07-31T02:42:41</t>
-        </is>
+      <c r="F260" s="2" t="n">
+        <v>45869.11297453703</v>
       </c>
       <c r="G260" t="inlineStr">
         <is>
@@ -9423,10 +8897,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F261" t="inlineStr">
-        <is>
-          <t>2025-07-30T18:09:29</t>
-        </is>
+      <c r="F261" s="2" t="n">
+        <v>45868.75658564815</v>
       </c>
       <c r="G261" t="inlineStr">
         <is>
@@ -9458,10 +8930,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F262" t="inlineStr">
-        <is>
-          <t>2026-02-04T12:20:19</t>
-        </is>
+      <c r="F262" s="2" t="n">
+        <v>46057.5141087963</v>
       </c>
       <c r="G262" t="inlineStr">
         <is>
@@ -9493,10 +8963,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F263" t="inlineStr">
-        <is>
-          <t>2026-01-16T17:19:06</t>
-        </is>
+      <c r="F263" s="2" t="n">
+        <v>46038.72159722223</v>
       </c>
       <c r="G263" t="inlineStr">
         <is>
@@ -9528,10 +8996,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F264" t="inlineStr">
-        <is>
-          <t>2026-02-11T10:49:40</t>
-        </is>
+      <c r="F264" s="2" t="n">
+        <v>46064.45115740741</v>
       </c>
       <c r="G264" t="inlineStr">
         <is>
@@ -9563,10 +9029,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F265" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:46:47</t>
-        </is>
+      <c r="F265" s="2" t="n">
+        <v>45868.65748842592</v>
       </c>
       <c r="G265" t="inlineStr">
         <is>
@@ -9598,10 +9062,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F266" t="inlineStr">
-        <is>
-          <t>2025-08-21T10:46:28</t>
-        </is>
+      <c r="F266" s="2" t="n">
+        <v>45890.44893518519</v>
       </c>
       <c r="G266" t="inlineStr">
         <is>
@@ -9633,10 +9095,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F267" t="inlineStr">
-        <is>
-          <t>2025-12-31T11:37:33</t>
-        </is>
+      <c r="F267" s="2" t="n">
+        <v>46022.48440972222</v>
       </c>
       <c r="G267" t="inlineStr">
         <is>
@@ -9668,10 +9128,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F268" t="inlineStr">
-        <is>
-          <t>2026-02-12T14:44:37</t>
-        </is>
+      <c r="F268" s="2" t="n">
+        <v>46065.61431712963</v>
       </c>
       <c r="G268" t="inlineStr">
         <is>
@@ -9703,10 +9161,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F269" t="inlineStr">
-        <is>
-          <t>2026-01-24T18:31:46</t>
-        </is>
+      <c r="F269" s="2" t="n">
+        <v>46046.77206018518</v>
       </c>
       <c r="G269" t="inlineStr">
         <is>
@@ -9738,10 +9194,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F270" t="inlineStr">
-        <is>
-          <t>2025-07-31T09:10:05</t>
-        </is>
+      <c r="F270" s="2" t="n">
+        <v>45869.38200231481</v>
       </c>
       <c r="G270" t="inlineStr">
         <is>
@@ -9773,10 +9227,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F271" t="inlineStr">
-        <is>
-          <t>2025-11-10T07:50:50</t>
-        </is>
+      <c r="F271" s="2" t="n">
+        <v>45971.32696759259</v>
       </c>
       <c r="G271" t="inlineStr">
         <is>
@@ -9808,10 +9260,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F272" t="inlineStr">
-        <is>
-          <t>2026-01-14T19:23:14</t>
-        </is>
+      <c r="F272" s="2" t="n">
+        <v>46036.80780092593</v>
       </c>
       <c r="G272" t="inlineStr">
         <is>
@@ -9843,10 +9293,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F273" t="inlineStr">
-        <is>
-          <t>2025-07-30T19:06:35</t>
-        </is>
+      <c r="F273" s="2" t="n">
+        <v>45868.79623842592</v>
       </c>
       <c r="G273" t="inlineStr">
         <is>
@@ -9878,10 +9326,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F274" t="inlineStr">
-        <is>
-          <t>2026-01-23T22:45:17</t>
-        </is>
+      <c r="F274" s="2" t="n">
+        <v>46045.94811342593</v>
       </c>
       <c r="G274" t="inlineStr">
         <is>
@@ -9913,10 +9359,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F275" t="inlineStr">
-        <is>
-          <t>2025-08-19T06:18:01</t>
-        </is>
+      <c r="F275" s="2" t="n">
+        <v>45888.26251157407</v>
       </c>
     </row>
     <row r="276">
@@ -9943,10 +9387,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F276" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:43:03</t>
-        </is>
+      <c r="F276" s="2" t="n">
+        <v>45868.6965625</v>
       </c>
       <c r="G276" t="inlineStr">
         <is>
@@ -9978,10 +9420,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F277" t="inlineStr">
-        <is>
-          <t>2026-01-20T15:37:11</t>
-        </is>
+      <c r="F277" s="2" t="n">
+        <v>46042.65082175926</v>
       </c>
       <c r="G277" t="inlineStr">
         <is>
@@ -10013,10 +9453,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F278" t="inlineStr">
-        <is>
-          <t>2026-01-28T14:41:57</t>
-        </is>
+      <c r="F278" s="2" t="n">
+        <v>46050.61246527778</v>
       </c>
       <c r="G278" t="inlineStr">
         <is>
@@ -10048,10 +9486,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F279" t="inlineStr">
-        <is>
-          <t>2026-02-11T11:00:28</t>
-        </is>
+      <c r="F279" s="2" t="n">
+        <v>46064.45865740741</v>
       </c>
       <c r="G279" t="inlineStr">
         <is>
@@ -10083,10 +9519,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F280" t="inlineStr">
-        <is>
-          <t>2026-02-19T18:27:43</t>
-        </is>
+      <c r="F280" s="2" t="n">
+        <v>46072.76924768519</v>
       </c>
       <c r="G280" t="inlineStr">
         <is>
@@ -10118,10 +9552,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F281" t="inlineStr">
-        <is>
-          <t>2026-02-19T19:38:36</t>
-        </is>
+      <c r="F281" s="2" t="n">
+        <v>46072.81847222222</v>
       </c>
       <c r="G281" t="inlineStr">
         <is>
@@ -10153,10 +9585,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F282" t="inlineStr">
-        <is>
-          <t>2026-02-12T16:16:03</t>
-        </is>
+      <c r="F282" s="2" t="n">
+        <v>46065.6778125</v>
       </c>
       <c r="G282" t="inlineStr">
         <is>
@@ -10188,10 +9618,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F283" t="inlineStr">
-        <is>
-          <t>2025-12-01T13:57:55</t>
-        </is>
+      <c r="F283" s="2" t="n">
+        <v>45992.58188657407</v>
       </c>
       <c r="G283" t="inlineStr">
         <is>
@@ -10223,10 +9651,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F284" t="inlineStr">
-        <is>
-          <t>2025-09-02T15:51:58</t>
-        </is>
+      <c r="F284" s="2" t="n">
+        <v>45902.66108796297</v>
       </c>
       <c r="G284" t="inlineStr">
         <is>
@@ -10258,10 +9684,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F285" t="inlineStr">
-        <is>
-          <t>2026-02-07T09:20:58</t>
-        </is>
+      <c r="F285" s="2" t="n">
+        <v>46060.38956018518</v>
       </c>
       <c r="G285" t="inlineStr">
         <is>
@@ -10293,10 +9717,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F286" t="inlineStr">
-        <is>
-          <t>2026-02-04T11:08:06</t>
-        </is>
+      <c r="F286" s="2" t="n">
+        <v>46057.46395833333</v>
       </c>
       <c r="G286" t="inlineStr">
         <is>
@@ -10328,10 +9750,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F287" t="inlineStr">
-        <is>
-          <t>2025-07-31T15:40:04</t>
-        </is>
+      <c r="F287" s="2" t="n">
+        <v>45869.65282407407</v>
       </c>
       <c r="G287" t="inlineStr">
         <is>
@@ -10363,10 +9783,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F288" t="inlineStr">
-        <is>
-          <t>2025-07-31T08:19:32</t>
-        </is>
+      <c r="F288" s="2" t="n">
+        <v>45869.34689814815</v>
       </c>
     </row>
     <row r="289">
@@ -10393,10 +9811,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F289" t="inlineStr">
-        <is>
-          <t>2025-12-22T11:13:23</t>
-        </is>
+      <c r="F289" s="2" t="n">
+        <v>46013.46762731481</v>
       </c>
       <c r="G289" t="inlineStr">
         <is>
@@ -10428,10 +9844,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F290" t="inlineStr">
-        <is>
-          <t>2025-09-04T11:13:10</t>
-        </is>
+      <c r="F290" s="2" t="n">
+        <v>45904.46747685185</v>
       </c>
       <c r="G290" t="inlineStr">
         <is>
@@ -10463,10 +9877,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F291" t="inlineStr">
-        <is>
-          <t>2026-02-03T14:39:33</t>
-        </is>
+      <c r="F291" s="2" t="n">
+        <v>46056.61079861111</v>
       </c>
       <c r="G291" t="inlineStr">
         <is>
@@ -10498,10 +9910,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F292" t="inlineStr">
-        <is>
-          <t>2026-02-10T11:04:15</t>
-        </is>
+      <c r="F292" s="2" t="n">
+        <v>46063.46128472222</v>
       </c>
       <c r="G292" t="inlineStr">
         <is>
@@ -10533,10 +9943,8 @@
           <t>Em manutenção</t>
         </is>
       </c>
-      <c r="F293" t="inlineStr">
-        <is>
-          <t>2025-10-03T11:32:11</t>
-        </is>
+      <c r="F293" s="2" t="n">
+        <v>45933.48068287037</v>
       </c>
     </row>
     <row r="294">
@@ -10563,10 +9971,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F294" t="inlineStr">
-        <is>
-          <t>2026-01-08T22:41:31</t>
-        </is>
+      <c r="F294" s="2" t="n">
+        <v>46030.94549768518</v>
       </c>
       <c r="G294" t="inlineStr">
         <is>
@@ -10598,10 +10004,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F295" t="inlineStr">
-        <is>
-          <t>2025-11-24T08:01:25</t>
-        </is>
+      <c r="F295" s="2" t="n">
+        <v>45985.33431712963</v>
       </c>
       <c r="G295" t="inlineStr">
         <is>
@@ -10633,10 +10037,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F296" t="inlineStr">
-        <is>
-          <t>2025-07-31T02:06:59</t>
-        </is>
+      <c r="F296" s="2" t="n">
+        <v>45869.08818287037</v>
       </c>
     </row>
     <row r="297">
@@ -10663,10 +10065,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F297" t="inlineStr">
-        <is>
-          <t>2025-07-31T12:38:43</t>
-        </is>
+      <c r="F297" s="2" t="n">
+        <v>45869.52688657407</v>
       </c>
       <c r="G297" t="inlineStr">
         <is>
@@ -10698,10 +10098,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F298" t="inlineStr">
-        <is>
-          <t>2025-12-11T08:38:58</t>
-        </is>
+      <c r="F298" s="2" t="n">
+        <v>46002.36039351852</v>
       </c>
     </row>
     <row r="299">
@@ -10728,10 +10126,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F299" t="inlineStr">
-        <is>
-          <t>2026-02-02T10:29:37</t>
-        </is>
+      <c r="F299" s="2" t="n">
+        <v>46055.4372337963</v>
       </c>
       <c r="G299" t="inlineStr">
         <is>
@@ -10763,10 +10159,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F300" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:50:40</t>
-        </is>
+      <c r="F300" s="2" t="n">
+        <v>45868.66018518519</v>
       </c>
       <c r="G300" t="inlineStr">
         <is>
@@ -10798,10 +10192,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F301" t="inlineStr">
-        <is>
-          <t>2026-02-13T13:33:59</t>
-        </is>
+      <c r="F301" s="2" t="n">
+        <v>46066.5652662037</v>
       </c>
       <c r="G301" t="inlineStr">
         <is>
@@ -10833,10 +10225,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F302" t="inlineStr">
-        <is>
-          <t>2025-09-30T18:52:31</t>
-        </is>
+      <c r="F302" s="2" t="n">
+        <v>45930.78646990741</v>
       </c>
     </row>
     <row r="303">
@@ -10863,10 +10253,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F303" t="inlineStr">
-        <is>
-          <t>2026-02-11T15:42:16</t>
-        </is>
+      <c r="F303" s="2" t="n">
+        <v>46064.65435185185</v>
       </c>
     </row>
     <row r="304">
@@ -10893,10 +10281,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F304" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:32:12</t>
-        </is>
+      <c r="F304" s="2" t="n">
+        <v>45868.68902777778</v>
       </c>
       <c r="G304" t="inlineStr">
         <is>
@@ -10928,10 +10314,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F305" t="inlineStr">
-        <is>
-          <t>2025-12-24T08:03:49</t>
-        </is>
+      <c r="F305" s="2" t="n">
+        <v>46015.3359837963</v>
       </c>
       <c r="G305" t="inlineStr">
         <is>
@@ -10963,10 +10347,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F306" t="inlineStr">
-        <is>
-          <t>2026-02-19T10:34:43</t>
-        </is>
+      <c r="F306" s="2" t="n">
+        <v>46072.44077546296</v>
       </c>
       <c r="G306" t="inlineStr">
         <is>
@@ -10998,10 +10380,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F307" t="inlineStr">
-        <is>
-          <t>2025-07-31T14:46:08</t>
-        </is>
+      <c r="F307" s="2" t="n">
+        <v>45869.61537037037</v>
       </c>
       <c r="G307" t="inlineStr">
         <is>
@@ -11033,10 +10413,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F308" t="inlineStr">
-        <is>
-          <t>2025-07-31T12:42:49</t>
-        </is>
+      <c r="F308" s="2" t="n">
+        <v>45869.5297337963</v>
       </c>
       <c r="G308" t="inlineStr">
         <is>
@@ -11068,10 +10446,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F309" t="inlineStr">
-        <is>
-          <t>2026-02-11T13:36:13</t>
-        </is>
+      <c r="F309" s="2" t="n">
+        <v>46064.56681712963</v>
       </c>
       <c r="G309" t="inlineStr">
         <is>
@@ -11103,10 +10479,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F310" t="inlineStr">
-        <is>
-          <t>2026-02-19T10:47:19</t>
-        </is>
+      <c r="F310" s="2" t="n">
+        <v>46072.44952546297</v>
       </c>
       <c r="G310" t="inlineStr">
         <is>
@@ -11138,10 +10512,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F311" t="inlineStr">
-        <is>
-          <t>2025-07-30T17:00:04</t>
-        </is>
+      <c r="F311" s="2" t="n">
+        <v>45868.70837962963</v>
       </c>
       <c r="G311" t="inlineStr">
         <is>
@@ -11173,10 +10545,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F312" t="inlineStr">
-        <is>
-          <t>2025-08-01T10:31:30</t>
-        </is>
+      <c r="F312" s="2" t="n">
+        <v>45870.43854166667</v>
       </c>
       <c r="G312" t="inlineStr">
         <is>
@@ -11208,10 +10578,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F313" t="inlineStr">
-        <is>
-          <t>2026-02-03T11:56:41</t>
-        </is>
+      <c r="F313" s="2" t="n">
+        <v>46056.49769675926</v>
       </c>
       <c r="G313" t="inlineStr">
         <is>
@@ -11243,10 +10611,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F314" t="inlineStr">
-        <is>
-          <t>2025-11-17T09:07:46</t>
-        </is>
+      <c r="F314" s="2" t="n">
+        <v>45978.38039351852</v>
       </c>
       <c r="G314" t="inlineStr">
         <is>
@@ -11278,10 +10644,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F315" t="inlineStr">
-        <is>
-          <t>2025-07-31T19:48:36</t>
-        </is>
+      <c r="F315" s="2" t="n">
+        <v>45869.82541666667</v>
       </c>
       <c r="G315" t="inlineStr">
         <is>
@@ -11313,10 +10677,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F316" t="inlineStr">
-        <is>
-          <t>2026-02-10T10:39:45</t>
-        </is>
+      <c r="F316" s="2" t="n">
+        <v>46063.44427083333</v>
       </c>
       <c r="G316" t="inlineStr">
         <is>
@@ -11348,10 +10710,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F317" t="inlineStr">
-        <is>
-          <t>2025-07-31T11:01:43</t>
-        </is>
+      <c r="F317" s="2" t="n">
+        <v>45869.45952546296</v>
       </c>
       <c r="G317" t="inlineStr">
         <is>
@@ -11383,10 +10743,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F318" t="inlineStr">
-        <is>
-          <t>2025-07-31T16:47:43</t>
-        </is>
+      <c r="F318" s="2" t="n">
+        <v>45869.69980324074</v>
       </c>
       <c r="G318" t="inlineStr">
         <is>
@@ -11418,10 +10776,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F319" t="inlineStr">
-        <is>
-          <t>2025-11-12T14:53:54</t>
-        </is>
+      <c r="F319" s="2" t="n">
+        <v>45973.62076388889</v>
       </c>
       <c r="G319" t="inlineStr">
         <is>
@@ -11453,10 +10809,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F320" t="inlineStr">
-        <is>
-          <t>2025-07-31T07:55:03</t>
-        </is>
+      <c r="F320" s="2" t="n">
+        <v>45869.32989583333</v>
       </c>
       <c r="G320" t="inlineStr">
         <is>
@@ -11488,10 +10842,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F321" t="inlineStr">
-        <is>
-          <t>2025-09-20T09:36:58</t>
-        </is>
+      <c r="F321" s="2" t="n">
+        <v>45920.40067129629</v>
       </c>
       <c r="G321" t="inlineStr">
         <is>
@@ -11523,10 +10875,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F322" t="inlineStr">
-        <is>
-          <t>2025-09-05T14:18:33</t>
-        </is>
+      <c r="F322" s="2" t="n">
+        <v>45905.59621527778</v>
       </c>
       <c r="G322" t="inlineStr">
         <is>
@@ -11558,10 +10908,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F323" t="inlineStr">
-        <is>
-          <t>2025-07-31T15:40:04</t>
-        </is>
+      <c r="F323" s="2" t="n">
+        <v>45869.65282407407</v>
       </c>
       <c r="G323" t="inlineStr">
         <is>
@@ -11593,10 +10941,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F324" t="inlineStr">
-        <is>
-          <t>2026-01-13T15:29:39</t>
-        </is>
+      <c r="F324" s="2" t="n">
+        <v>46035.64559027777</v>
       </c>
       <c r="G324" t="inlineStr">
         <is>
@@ -11628,10 +10974,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F325" t="inlineStr">
-        <is>
-          <t>2026-01-08T09:48:54</t>
-        </is>
+      <c r="F325" s="2" t="n">
+        <v>46030.40895833333</v>
       </c>
       <c r="G325" t="inlineStr">
         <is>
@@ -11663,10 +11007,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F326" t="inlineStr">
-        <is>
-          <t>2026-02-19T09:25:26</t>
-        </is>
+      <c r="F326" s="2" t="n">
+        <v>46072.39266203704</v>
       </c>
       <c r="G326" t="inlineStr">
         <is>
@@ -11698,10 +11040,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F327" t="inlineStr">
-        <is>
-          <t>2025-10-07T10:13:24</t>
-        </is>
+      <c r="F327" s="2" t="n">
+        <v>45937.42597222222</v>
       </c>
     </row>
     <row r="328">
@@ -11728,10 +11068,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F328" t="inlineStr">
-        <is>
-          <t>2026-02-13T08:14:44</t>
-        </is>
+      <c r="F328" s="2" t="n">
+        <v>46066.34356481482</v>
       </c>
       <c r="G328" t="inlineStr">
         <is>
@@ -11763,10 +11101,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F329" t="inlineStr">
-        <is>
-          <t>2026-02-07T09:58:16</t>
-        </is>
+      <c r="F329" s="2" t="n">
+        <v>46060.41546296296</v>
       </c>
       <c r="G329" t="inlineStr">
         <is>
@@ -11798,10 +11134,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F330" t="inlineStr">
-        <is>
-          <t>2025-07-31T07:57:03</t>
-        </is>
+      <c r="F330" s="2" t="n">
+        <v>45869.33128472222</v>
       </c>
       <c r="G330" t="inlineStr">
         <is>
@@ -11833,10 +11167,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F331" t="inlineStr">
-        <is>
-          <t>2026-01-20T11:33:21</t>
-        </is>
+      <c r="F331" s="2" t="n">
+        <v>46042.48149305556</v>
       </c>
       <c r="G331" t="inlineStr">
         <is>
@@ -11868,10 +11200,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F332" t="inlineStr">
-        <is>
-          <t>2025-07-30T15:20:13</t>
-        </is>
+      <c r="F332" s="2" t="n">
+        <v>45868.63903935185</v>
       </c>
       <c r="G332" t="inlineStr">
         <is>
@@ -11903,10 +11233,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F333" t="inlineStr">
-        <is>
-          <t>2026-01-23T11:19:59</t>
-        </is>
+      <c r="F333" s="2" t="n">
+        <v>46045.47221064815</v>
       </c>
       <c r="G333" t="inlineStr">
         <is>
@@ -11938,10 +11266,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F334" t="inlineStr">
-        <is>
-          <t>2026-01-30T16:01:17</t>
-        </is>
+      <c r="F334" s="2" t="n">
+        <v>46052.66755787037</v>
       </c>
       <c r="G334" t="inlineStr">
         <is>
@@ -11973,10 +11299,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F335" t="inlineStr">
-        <is>
-          <t>2025-12-11T02:04:19</t>
-        </is>
+      <c r="F335" s="2" t="n">
+        <v>46002.08633101852</v>
       </c>
       <c r="G335" t="inlineStr">
         <is>
@@ -12008,10 +11332,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F336" t="inlineStr">
-        <is>
-          <t>2025-08-01T13:50:36</t>
-        </is>
+      <c r="F336" s="2" t="n">
+        <v>45870.57680555555</v>
       </c>
       <c r="G336" t="inlineStr">
         <is>
@@ -12043,10 +11365,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F337" t="inlineStr">
-        <is>
-          <t>2025-07-30T18:49:17</t>
-        </is>
+      <c r="F337" s="2" t="n">
+        <v>45868.78422453703</v>
       </c>
       <c r="G337" t="inlineStr">
         <is>
@@ -12078,10 +11398,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F338" t="inlineStr">
-        <is>
-          <t>2025-07-31T17:18:39</t>
-        </is>
+      <c r="F338" s="2" t="n">
+        <v>45869.72128472223</v>
       </c>
       <c r="G338" t="inlineStr">
         <is>
@@ -12113,10 +11431,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F339" t="inlineStr">
-        <is>
-          <t>2026-01-12T11:57:26</t>
-        </is>
+      <c r="F339" s="2" t="n">
+        <v>46034.49821759259</v>
       </c>
       <c r="G339" t="inlineStr">
         <is>
@@ -12148,10 +11464,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F340" t="inlineStr">
-        <is>
-          <t>2025-08-21T15:00:54</t>
-        </is>
+      <c r="F340" s="2" t="n">
+        <v>45890.625625</v>
       </c>
       <c r="G340" t="inlineStr">
         <is>
@@ -12183,10 +11497,8 @@
           <t>Ativo</t>
         </is>
       </c>
-      <c r="F341" t="inlineStr">
-        <is>
-          <t>2025-07-30T16:12:55</t>
-        </is>
+      <c r="F341" s="2" t="n">
+        <v>45868.67563657407</v>
       </c>
       <c r="G341" t="inlineStr">
         <is>

</xml_diff>